<commit_message>
Handle tabular parsing of CSV, TSV, and Excel.
</commit_message>
<xml_diff>
--- a/stemmarest/src/TestFiles/armexample.xlsx
+++ b/stemmarest/src/TestFiles/armexample.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,6 +95,22 @@
       <color theme="1"/>
       <name val="Sylfaen"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,14 +130,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,99 +479,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="17">
+    <row r="1" spans="1:3" ht="17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
       <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17">
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17">
+    </row>
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17">
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="17">
+    </row>
+    <row r="7" spans="1:3" ht="17">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17">
+    <row r="8" spans="1:3" ht="17">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17">
+    <row r="9" spans="1:3" ht="17">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>